<commit_message>
Implement and benchmark faster totient_sum
</commit_message>
<xml_diff>
--- a/src/number_benchmarks.xlsx
+++ b/src/number_benchmarks.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
   <si>
     <t xml:space="preserve">n</t>
   </si>
@@ -70,10 +70,13 @@
     <t xml:space="preserve">laptop</t>
   </si>
   <si>
+    <t xml:space="preserve">python 3.5</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.90</t>
   </si>
   <si>
-    <t xml:space="preserve">pypy</t>
+    <t xml:space="preserve">pypy 5.1.2</t>
   </si>
   <si>
     <t xml:space="preserve">1.30</t>
@@ -83,6 +86,48 @@
   </si>
   <si>
     <t xml:space="preserve">35.39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">totient_sum </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.092</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">57.91</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.029</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.065</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.39</t>
   </si>
 </sst>
 </file>
@@ -197,10 +242,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -277,8 +322,8 @@
       <c r="B3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="1" t="n">
-        <v>3.5</v>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="G3" s="1" t="n">
         <v>0.018</v>
@@ -287,7 +332,7 @@
         <v>0.17</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J3" s="1" t="n">
         <v>3.69</v>
@@ -307,7 +352,7 @@
         <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G4" s="1" t="n">
         <v>0.016</v>
@@ -322,13 +367,74 @@
         <v>0.25</v>
       </c>
       <c r="K4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>20</v>
+      <c r="G6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>